<commit_message>
Foi inserido o pop-up de verificação caso os alunos da planilha constem no banco de dados
</commit_message>
<xml_diff>
--- a/src/renderer/templates/FormatoImportacaoAluno.xlsx
+++ b/src/renderer/templates/FormatoImportacaoAluno.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dona Etelvina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dilan</t>
   </si>
   <si>
     <t xml:space="preserve">Amarelo</t>
@@ -262,10 +268,10 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
@@ -470,13 +476,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>36346</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2"/>
@@ -1267,10 +1297,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="J7 B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.11"/>
@@ -1282,10 +1312,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>14</v>
@@ -1294,7 +1324,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,7 +1341,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>17</v>
@@ -1319,13 +1349,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>27</v>
@@ -1339,21 +1369,21 @@
         <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1375,10 +1405,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J7 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>